<commit_message>
Projects 3 & 4
</commit_message>
<xml_diff>
--- a/Project 2/Project 2.4/wolves_standard_stats_scouted.xlsx
+++ b/Project 2/Project 2.4/wolves_standard_stats_scouted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekchui/Documents/Programming/Personal/Projects/Football Analytics/Project 2/Project 2.4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A46006C-B2B4-9E4F-977A-11C09B434423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B34316-D98E-2945-A000-6AB5CFD81254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25480" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3440" yWindow="500" windowWidth="29280" windowHeight="18100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -733,7 +733,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y19" sqref="Y19"/>
+      <selection pane="topRight" activeCell="AF20" sqref="AF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>